<commit_message>
Updates to appendix tables
</commit_message>
<xml_diff>
--- a/final-outputs/Table E International.xlsx
+++ b/final-outputs/Table E International.xlsx
@@ -579,7 +579,7 @@
     <t>CFC exempt if country included in white list and not receiving special tax treatment or taxed subject to a corporate rate of more than 11.25%</t>
   </si>
   <si>
-    <t>CFC exempt if i) not an artificial arrangement or ii) accounting profits  below €750,000 or less than 10% of operating costs</t>
+    <t>CFC exempt if i) not an artificial arrangement or ii) accounting profits below €750,000 or less than 10% of operating costs</t>
   </si>
   <si>
     <t>CFC exempt if not an artificial arrangement</t>
@@ -591,7 +591,7 @@
     <t>CFC exempt if located in EEA country and not an artificial arrangement or located in tax treaty country</t>
   </si>
   <si>
-    <t>CFC exempt if located in EU and EEA countries and not an artificial arrangement
+    <t>CFC exempt if located in EU and EEA countries and not an artificial arrangement
 Other exemptions can apply</t>
   </si>
   <si>
@@ -673,7 +673,7 @@
 Interest deductions limited to the higher of 30% of EBITDA or €3 million (financial institutions exempt)</t>
   </si>
   <si>
-    <t>3:1 debt-to-equity ratio applies.</t>
+    <t>3:1 debt-to-equity ratio applies</t>
   </si>
   <si>
     <t>Interest deductions limited to the higher of €1 million or 30% of EBITDA</t>

</xml_diff>

<commit_message>
Re-do of output tables
</commit_message>
<xml_diff>
--- a/final-outputs/Table E International.xlsx
+++ b/final-outputs/Table E International.xlsx
@@ -579,7 +579,7 @@
     <t>CFC exempt if country included in white list and not receiving special tax treatment or taxed subject to a corporate rate of more than 11.25%</t>
   </si>
   <si>
-    <t>CFC exempt if i) not an artificial arrangement or ii) accounting profits  below €750,000 or less than 10% of operating costs</t>
+    <t>CFC exempt if i) not an artificial arrangement or ii) accounting profits below €750,000 or less than 10% of operating costs</t>
   </si>
   <si>
     <t>CFC exempt if not an artificial arrangement</t>
@@ -591,7 +591,7 @@
     <t>CFC exempt if located in EEA country and not an artificial arrangement or located in tax treaty country</t>
   </si>
   <si>
-    <t>CFC exempt if located in EU and EEA countries and not an artificial arrangement
+    <t>CFC exempt if located in EU and EEA countries and not an artificial arrangement
 Other exemptions can apply</t>
   </si>
   <si>
@@ -673,7 +673,7 @@
 Interest deductions limited to the higher of 30% of EBITDA or €3 million (financial institutions exempt)</t>
   </si>
   <si>
-    <t>3:1 debt-to-equity ratio applies.</t>
+    <t>3:1 debt-to-equity ratio applies</t>
   </si>
   <si>
     <t>Interest deductions limited to the higher of €1 million or 30% of EBITDA</t>

</xml_diff>

<commit_message>
Revert "Merge remote-tracking branch 'origin/README_updates' into README_updates_1"
This reverts commit bf495d931040ab195687288f9ec81397168ae2ff.
</commit_message>
<xml_diff>
--- a/final-outputs/Table E International.xlsx
+++ b/final-outputs/Table E International.xlsx
@@ -579,7 +579,7 @@
     <t>CFC exempt if country included in white list and not receiving special tax treatment or taxed subject to a corporate rate of more than 11.25%</t>
   </si>
   <si>
-    <t>CFC exempt if i) not an artificial arrangement or ii) accounting profits below €750,000 or less than 10% of operating costs</t>
+    <t>CFC exempt if i) not an artificial arrangement or ii) accounting profits  below €750,000 or less than 10% of operating costs</t>
   </si>
   <si>
     <t>CFC exempt if not an artificial arrangement</t>
@@ -591,7 +591,7 @@
     <t>CFC exempt if located in EEA country and not an artificial arrangement or located in tax treaty country</t>
   </si>
   <si>
-    <t>CFC exempt if located in EU and EEA countries and not an artificial arrangement
+    <t>CFC exempt if located in EU and EEA countries and not an artificial arrangement
 Other exemptions can apply</t>
   </si>
   <si>
@@ -673,7 +673,7 @@
 Interest deductions limited to the higher of 30% of EBITDA or €3 million (financial institutions exempt)</t>
   </si>
   <si>
-    <t>3:1 debt-to-equity ratio applies</t>
+    <t>3:1 debt-to-equity ratio applies.</t>
   </si>
   <si>
     <t>Interest deductions limited to the higher of €1 million or 30% of EBITDA</t>

</xml_diff>